<commit_message>
FSM seq no starts at 1 instead of 0
</commit_message>
<xml_diff>
--- a/part2a_results.xlsx
+++ b/part2a_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15880" tabRatio="991"/>
+    <workbookView xWindow="-8340" yWindow="0" windowWidth="25600" windowHeight="15880" tabRatio="991"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="15">
   <si>
     <t>window size</t>
   </si>
@@ -42,10 +42,40 @@
     <t>20ms</t>
   </si>
   <si>
-    <t>100ms</t>
+    <t>to find the retry timeout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>400ms</t>
+    <t>windowsize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>retrytimeout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>throughput</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>average</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -100,8 +130,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -180,7 +222,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="87">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
@@ -219,6 +261,12 @@
     <cellStyle name="已瀏覽過的超連結" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
@@ -256,10 +304,490 @@
     <cellStyle name="超連結" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="85" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$K$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$G$33:$G$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>160.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>180.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>200.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$K$33:$K$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>235.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>259.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>246.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>247.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>245.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>222.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>221.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>190.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>178.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>146.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>161.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>161.6666666666667</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>143.3333333333333</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2121376024"/>
+        <c:axId val="-2121348344"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2121376024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121348344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2121348344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121376024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>工作表1!$T$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>工作表1!$P$33:$P$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>工作表1!$T$33:$T$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>71.622</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.916</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.364</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74.646</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73.594</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72.404</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>71.369</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72.909</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68.423</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>72.651</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2116912648"/>
+        <c:axId val="-2116914072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2116912648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2116914072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2116914072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2116912648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="圖表 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="圖表 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -584,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -639,27 +1167,44 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>9.8379999999999992</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="M2">
+        <v>2.4820000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="C3">
+        <v>46.904000000000003</v>
+      </c>
+      <c r="H3">
+        <v>9.8680000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:14">
+      <c r="C4">
+        <v>46.972000000000001</v>
+      </c>
       <c r="D4">
         <f>AVERAGE(C2:C4)</f>
-        <v>47.454999999999998</v>
-      </c>
-      <c r="I4" t="e">
+        <v>47.110333333333337</v>
+      </c>
+      <c r="I4">
         <f>AVERAGE(H2:H4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N4" t="e">
+        <v>9.8529999999999998</v>
+      </c>
+      <c r="N4">
         <f>AVERAGE(M2:M4)</f>
-        <v>#DIV/0!</v>
+        <v>2.4820000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -669,31 +1214,54 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
+      <c r="C5">
+        <v>93.061999999999998</v>
+      </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>19.547999999999998</v>
       </c>
       <c r="K5">
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="M5">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="C6">
+        <v>93.436000000000007</v>
+      </c>
+      <c r="H6">
+        <v>19.533999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="D7" t="e">
+      <c r="C7">
+        <v>92.558999999999997</v>
+      </c>
+      <c r="D7">
         <f>AVERAGE(C5:C7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I7" t="e">
+        <v>93.019000000000005</v>
+      </c>
+      <c r="H7">
+        <v>19.521999999999998</v>
+      </c>
+      <c r="I7">
         <f>AVERAGE(H5:H7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N7" t="e">
+        <v>19.534666666666663</v>
+      </c>
+      <c r="N7">
         <f>AVERAGE(M5:M7)</f>
-        <v>#DIV/0!</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -703,31 +1271,54 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
+      <c r="C8">
+        <v>185.03200000000001</v>
+      </c>
       <c r="F8">
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>38.700000000000003</v>
       </c>
       <c r="K8">
         <v>4</v>
       </c>
       <c r="L8" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="M8">
+        <v>9.8670000000000009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="C9">
+        <v>183.595</v>
+      </c>
+      <c r="H9">
+        <v>38.816000000000003</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="D10" t="e">
+      <c r="C10">
+        <v>182.684</v>
+      </c>
+      <c r="D10">
         <f>AVERAGE(C8:C10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" t="e">
+        <v>183.77033333333335</v>
+      </c>
+      <c r="H10">
+        <v>39.204000000000001</v>
+      </c>
+      <c r="I10">
         <f>AVERAGE(H8:H10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N10" t="e">
+        <v>38.906666666666666</v>
+      </c>
+      <c r="N10">
         <f>AVERAGE(M8:M10)</f>
-        <v>#DIV/0!</v>
+        <v>9.8670000000000009</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -737,31 +1328,54 @@
       <c r="B11" t="s">
         <v>5</v>
       </c>
+      <c r="C11">
+        <v>324.68099999999998</v>
+      </c>
       <c r="F11">
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="H11">
+        <v>76.233999999999995</v>
       </c>
       <c r="K11">
         <v>8</v>
       </c>
       <c r="L11" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="M11">
+        <v>19.55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="C12">
+        <v>313.91899999999998</v>
+      </c>
+      <c r="H12">
+        <v>77.012</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="D13" t="e">
+      <c r="C13">
+        <v>331.089</v>
+      </c>
+      <c r="D13">
         <f>AVERAGE(C11:C13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I13" t="e">
+        <v>323.22966666666662</v>
+      </c>
+      <c r="H13">
+        <v>77.304000000000002</v>
+      </c>
+      <c r="I13">
         <f>AVERAGE(H11:H13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N13" t="e">
+        <v>76.849999999999994</v>
+      </c>
+      <c r="N13">
         <f>AVERAGE(M11:M13)</f>
-        <v>#DIV/0!</v>
+        <v>19.55</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -771,166 +1385,726 @@
       <c r="B14" t="s">
         <v>5</v>
       </c>
+      <c r="C14">
+        <v>450.745</v>
+      </c>
       <c r="F14">
         <v>16</v>
       </c>
       <c r="G14" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <v>144.09700000000001</v>
       </c>
       <c r="K14">
         <v>16</v>
       </c>
       <c r="L14" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="M14">
+        <v>38.573999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="C15">
+        <v>467.64499999999998</v>
+      </c>
+      <c r="H15">
+        <v>136.79300000000001</v>
+      </c>
+      <c r="M15">
+        <v>38.44</v>
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="D16" t="e">
+      <c r="C16">
+        <v>472.81799999999998</v>
+      </c>
+      <c r="D16">
         <f>AVERAGE(C14:C16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I16" t="e">
+        <v>463.73600000000005</v>
+      </c>
+      <c r="H16">
+        <v>139.345</v>
+      </c>
+      <c r="I16">
         <f>AVERAGE(H14:H16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" t="e">
+        <v>140.07833333333335</v>
+      </c>
+      <c r="N16">
         <f>AVERAGE(M14:M16)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>38.506999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
+      <c r="C17">
+        <v>497.81900000000002</v>
+      </c>
       <c r="F17">
         <v>32</v>
       </c>
       <c r="G17" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="H17">
+        <v>230.77600000000001</v>
       </c>
       <c r="K17">
         <v>32</v>
       </c>
       <c r="L17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="D19" t="e">
+        <v>14</v>
+      </c>
+      <c r="M17">
+        <v>73.209999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="C18">
+        <v>492.20400000000001</v>
+      </c>
+      <c r="H18">
+        <v>239.755</v>
+      </c>
+      <c r="M18">
+        <v>71.576999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="C19">
+        <v>578.93299999999999</v>
+      </c>
+      <c r="D19">
         <f>AVERAGE(C17:C19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I19" t="e">
+        <v>522.98533333333341</v>
+      </c>
+      <c r="H19">
+        <v>245.946</v>
+      </c>
+      <c r="I19">
         <f>AVERAGE(H17:H19)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N19" t="e">
+        <v>238.82566666666665</v>
+      </c>
+      <c r="M19">
+        <v>72.307000000000002</v>
+      </c>
+      <c r="N19">
         <f>AVERAGE(M17:M19)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>72.364666666666665</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20">
         <v>64</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
+      <c r="C20">
+        <v>336.15100000000001</v>
+      </c>
       <c r="F20">
         <v>64</v>
       </c>
       <c r="G20" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="H20">
+        <v>218.21899999999999</v>
       </c>
       <c r="K20">
         <v>64</v>
       </c>
       <c r="L20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="D22" t="e">
+        <v>14</v>
+      </c>
+      <c r="M20">
+        <v>91.11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="C21">
+        <v>342.887</v>
+      </c>
+      <c r="H21">
+        <v>227.21199999999999</v>
+      </c>
+      <c r="M21">
+        <v>87.08</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="C22">
+        <v>363.87799999999999</v>
+      </c>
+      <c r="D22">
         <f>AVERAGE(C20:C22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" t="e">
+        <v>347.63866666666667</v>
+      </c>
+      <c r="H22">
+        <v>226.553</v>
+      </c>
+      <c r="I22">
         <f>AVERAGE(H20:H22)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N22" t="e">
+        <v>223.99466666666663</v>
+      </c>
+      <c r="N22">
         <f>AVERAGE(M20:M22)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>89.094999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
       <c r="A23">
         <v>128</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
+      <c r="C23">
+        <v>258.19299999999998</v>
+      </c>
       <c r="F23">
         <v>128</v>
       </c>
       <c r="G23" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="H23">
+        <v>263.15899999999999</v>
       </c>
       <c r="K23">
         <v>128</v>
       </c>
       <c r="L23" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="D25" t="e">
+        <v>14</v>
+      </c>
+      <c r="M23">
+        <v>87.87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="C24">
+        <v>246.15899999999999</v>
+      </c>
+      <c r="H24">
+        <v>221.56</v>
+      </c>
+      <c r="M24">
+        <v>91.623000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="C25">
+        <v>261.43799999999999</v>
+      </c>
+      <c r="D25">
         <f>AVERAGE(C23:C25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" t="e">
+        <v>255.26333333333332</v>
+      </c>
+      <c r="H25">
+        <v>253.70500000000001</v>
+      </c>
+      <c r="I25">
         <f>AVERAGE(H23:H25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N25" t="e">
+        <v>246.14133333333334</v>
+      </c>
+      <c r="M25">
+        <v>91.698999999999998</v>
+      </c>
+      <c r="N25">
         <f>AVERAGE(M23:M25)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+        <v>90.397333333333336</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26">
         <v>256</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
+      <c r="C26">
+        <v>305.66899999999998</v>
+      </c>
       <c r="F26">
         <v>256</v>
       </c>
       <c r="G26" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="H26">
+        <v>223.90600000000001</v>
       </c>
       <c r="K26">
         <v>256</v>
       </c>
       <c r="L26" t="s">
+        <v>14</v>
+      </c>
+      <c r="M26">
+        <v>88.515000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="C27">
+        <v>299.11599999999999</v>
+      </c>
+      <c r="H27">
+        <v>224.61600000000001</v>
+      </c>
+      <c r="M27">
+        <v>89.914000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="C28">
+        <v>274.33800000000002</v>
+      </c>
+      <c r="D28">
+        <f>AVERAGE(C26:C28)</f>
+        <v>293.041</v>
+      </c>
+      <c r="H28">
+        <v>232.31</v>
+      </c>
+      <c r="I28">
+        <f>AVERAGE(H26:H28)</f>
+        <v>226.94400000000005</v>
+      </c>
+      <c r="M28">
+        <v>101.354</v>
+      </c>
+      <c r="N28">
+        <f>AVERAGE(M26:M28)</f>
+        <v>93.26100000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" t="s">
+        <v>10</v>
+      </c>
+      <c r="O31" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="F32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="D28" t="e">
-        <f>AVERAGE(C26:C28)</f>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" t="s">
+        <v>11</v>
+      </c>
+      <c r="O32" t="s">
+        <v>7</v>
+      </c>
+      <c r="P32" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>9</v>
+      </c>
+      <c r="T32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="6:20">
+      <c r="F33">
+        <v>32</v>
+      </c>
+      <c r="G33">
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <v>238</v>
+      </c>
+      <c r="I33">
+        <v>233</v>
+      </c>
+      <c r="K33">
+        <f>AVERAGE(H33:J33)</f>
+        <v>235.5</v>
+      </c>
+      <c r="O33">
+        <v>32</v>
+      </c>
+      <c r="P33">
+        <v>10</v>
+      </c>
+      <c r="Q33">
+        <v>71.622</v>
+      </c>
+      <c r="T33">
+        <f>AVERAGE(Q33:S33)</f>
+        <v>71.622</v>
+      </c>
+    </row>
+    <row r="34" spans="6:20">
+      <c r="G34">
+        <v>20</v>
+      </c>
+      <c r="H34">
+        <v>262</v>
+      </c>
+      <c r="I34">
+        <v>249</v>
+      </c>
+      <c r="J34">
+        <v>266</v>
+      </c>
+      <c r="K34">
+        <f t="shared" ref="K34:K51" si="0">AVERAGE(H34:J34)</f>
+        <v>259</v>
+      </c>
+      <c r="P34">
+        <v>20</v>
+      </c>
+      <c r="Q34">
+        <v>72.92</v>
+      </c>
+      <c r="T34">
+        <f t="shared" ref="T34:T45" si="1">AVERAGE(Q34:S34)</f>
+        <v>72.92</v>
+      </c>
+    </row>
+    <row r="35" spans="6:20">
+      <c r="G35">
+        <v>30</v>
+      </c>
+      <c r="H35">
+        <v>247</v>
+      </c>
+      <c r="I35">
+        <v>243</v>
+      </c>
+      <c r="J35">
+        <v>248</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>246</v>
+      </c>
+      <c r="P35">
+        <v>30</v>
+      </c>
+      <c r="Q35">
+        <v>74.915999999999997</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="1"/>
+        <v>74.915999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="6:20">
+      <c r="G36">
+        <v>40</v>
+      </c>
+      <c r="H36">
+        <v>244</v>
+      </c>
+      <c r="I36">
+        <v>259</v>
+      </c>
+      <c r="J36">
+        <v>238</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="0"/>
+        <v>247</v>
+      </c>
+      <c r="P36">
+        <v>40</v>
+      </c>
+      <c r="Q36">
+        <v>74.364000000000004</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="1"/>
+        <v>74.364000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="6:20">
+      <c r="G37">
+        <v>50</v>
+      </c>
+      <c r="H37">
+        <v>232</v>
+      </c>
+      <c r="I37">
+        <v>237</v>
+      </c>
+      <c r="J37">
+        <v>266</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="0"/>
+        <v>245</v>
+      </c>
+      <c r="P37">
+        <v>50</v>
+      </c>
+      <c r="Q37">
+        <v>72.23</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="1"/>
+        <v>72.23</v>
+      </c>
+    </row>
+    <row r="38" spans="6:20">
+      <c r="G38">
+        <v>60</v>
+      </c>
+      <c r="H38">
+        <v>227</v>
+      </c>
+      <c r="I38">
+        <v>210</v>
+      </c>
+      <c r="J38">
+        <v>230</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="0"/>
+        <v>222.33333333333334</v>
+      </c>
+      <c r="P38">
+        <v>60</v>
+      </c>
+      <c r="Q38">
+        <v>74.646000000000001</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="1"/>
+        <v>74.646000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="6:20">
+      <c r="G39">
+        <v>80</v>
+      </c>
+      <c r="H39">
+        <v>199</v>
+      </c>
+      <c r="I39">
+        <v>233</v>
+      </c>
+      <c r="J39">
+        <v>231</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="0"/>
+        <v>221</v>
+      </c>
+      <c r="P39">
+        <v>70</v>
+      </c>
+      <c r="Q39">
+        <v>73.593999999999994</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="1"/>
+        <v>73.593999999999994</v>
+      </c>
+    </row>
+    <row r="40" spans="6:20">
+      <c r="G40">
+        <v>100</v>
+      </c>
+      <c r="H40">
+        <v>175</v>
+      </c>
+      <c r="I40">
+        <v>223</v>
+      </c>
+      <c r="J40">
+        <v>172</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="0"/>
+        <v>190</v>
+      </c>
+      <c r="P40">
+        <v>80</v>
+      </c>
+      <c r="Q40">
+        <v>72.403999999999996</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="1"/>
+        <v>72.403999999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="6:20">
+      <c r="G41">
+        <v>120</v>
+      </c>
+      <c r="H41">
+        <v>178</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="0"/>
+        <v>178</v>
+      </c>
+      <c r="P41">
+        <v>100</v>
+      </c>
+      <c r="Q41">
+        <v>71.369</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="1"/>
+        <v>71.369</v>
+      </c>
+    </row>
+    <row r="42" spans="6:20">
+      <c r="G42">
+        <v>140</v>
+      </c>
+      <c r="H42">
+        <v>146</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="0"/>
+        <v>146</v>
+      </c>
+      <c r="P42">
+        <v>120</v>
+      </c>
+      <c r="Q42">
+        <v>72.909000000000006</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="1"/>
+        <v>72.909000000000006</v>
+      </c>
+    </row>
+    <row r="43" spans="6:20">
+      <c r="G43">
+        <v>160</v>
+      </c>
+      <c r="H43">
+        <v>161</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="0"/>
+        <v>161</v>
+      </c>
+      <c r="P43">
+        <v>150</v>
+      </c>
+      <c r="Q43">
+        <v>62.872999999999998</v>
+      </c>
+      <c r="R43">
+        <v>72.396000000000001</v>
+      </c>
+      <c r="S43">
+        <v>70</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="1"/>
+        <v>68.423000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="6:20">
+      <c r="G44">
+        <v>180</v>
+      </c>
+      <c r="H44">
+        <v>159</v>
+      </c>
+      <c r="I44">
+        <v>166</v>
+      </c>
+      <c r="J44">
+        <v>160</v>
+      </c>
+      <c r="K44">
+        <f>AVERAGE(H44:J44)</f>
+        <v>161.66666666666666</v>
+      </c>
+      <c r="P44">
+        <v>160</v>
+      </c>
+      <c r="Q44">
+        <v>72.650999999999996</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="1"/>
+        <v>72.650999999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="6:20">
+      <c r="G45">
+        <v>200</v>
+      </c>
+      <c r="H45">
+        <v>146</v>
+      </c>
+      <c r="I45">
+        <v>145</v>
+      </c>
+      <c r="J45">
+        <v>139</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="0"/>
+        <v>143.33333333333334</v>
+      </c>
+    </row>
+    <row r="46" spans="6:20">
+      <c r="K46" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="I28" t="e">
-        <f>AVERAGE(H26:H28)</f>
+    </row>
+    <row r="47" spans="6:20">
+      <c r="K47" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="N28" t="e">
-        <f>AVERAGE(M26:M28)</f>
+    </row>
+    <row r="48" spans="6:20">
+      <c r="K48" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="11:11">
+      <c r="K49" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="11:11">
+      <c r="K50" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="11:11">
+      <c r="K51" t="e">
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -938,6 +2112,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>